<commit_message>
Proceso de creacion y restablecimiento de Feature terminado
</commit_message>
<xml_diff>
--- a/DataEntry/Prueba.xlsx
+++ b/DataEntry/Prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Camiloch\Workspace\DataEntrySerenity\DataEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CCEFFD-8EC0-4209-B621-28D4B7745CAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5EA137-E28C-47BE-BE66-2ED7464E94BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prueba" sheetId="1" r:id="rId1"/>
@@ -899,11 +899,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -958,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538655B4-9915-4303-99A7-ED7BB241154A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
termina proyecto dataentry desde excel para serenity
</commit_message>
<xml_diff>
--- a/DataEntry/Prueba.xlsx
+++ b/DataEntry/Prueba.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Camiloch\Workspace\DataEntrySerenity\DataEntry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\DataentrySerenity\DataEntrySerenity\DataEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5EA137-E28C-47BE-BE66-2ED7464E94BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCE2541-D2A6-4F17-8428-7C3835B196C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prueba" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>CamiloCh</t>
+  </si>
+  <si>
+    <t>azxs1234</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -32,38 +45,29 @@
     <t>send</t>
   </si>
   <si>
-    <t>Camilo Chaparro</t>
-  </si>
-  <si>
-    <t>tarjeta debito</t>
-  </si>
-  <si>
-    <t>Diana Camila Ch</t>
-  </si>
-  <si>
-    <t>tarjeta credito</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Cta Ahorros</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>Camio</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>credito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +198,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -540,8 +552,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,62 +909,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538655B4-9915-4303-99A7-ED7BB241154A}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>3555648</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -960,35 +940,249 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538655B4-9915-4303-99A7-ED7BB241154A}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFD9ADA-7FAB-40DB-918F-21B41F2D51A9}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D622F5E4-10E3-4F97-8583-D4D1F08519A9}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>